<commit_message>
iaas summer school added
iaas summer school added
</commit_message>
<xml_diff>
--- a/Asunaro Summer 2015/Summer Schedule english2015.xlsx
+++ b/Asunaro Summer 2015/Summer Schedule english2015.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="24900" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -100,15 +105,9 @@
     <t>We are pirates!</t>
   </si>
   <si>
-    <t xml:space="preserve">Let's play Split the watermellon </t>
-  </si>
-  <si>
     <t>Swimming Petting Zoo</t>
   </si>
   <si>
-    <t>*Schedule may  change.</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
@@ -121,18 +120,6 @@
     <t>8/2</t>
   </si>
   <si>
-    <t>Week 3&amp;4 (7/6-7/17): Under The Sea</t>
-  </si>
-  <si>
-    <t>Week 7&amp;8  (8/3- 8/14): IAAS Circus</t>
-  </si>
-  <si>
-    <t>Let's go to     Under       the Sea</t>
-  </si>
-  <si>
-    <t>Week 5 &amp;6 (7/20-7/31): Japanese Festival!</t>
-  </si>
-  <si>
     <t>Let's make shaved ice</t>
   </si>
   <si>
@@ -163,14 +150,32 @@
     <t>Summer School Schedule 2015</t>
   </si>
   <si>
-    <t>Week 1&amp;2 (6/22-7/2):  Let's learn about America &amp;Tanabata Festival</t>
+    <t>Week 5 &amp; 6 (7/20-7/31): Matsuri - Japanese Festival!</t>
+  </si>
+  <si>
+    <t>Week 1 &amp; 2 (6/22-7/2):  Let's learn about America &amp;Tanabata Festival</t>
+  </si>
+  <si>
+    <t>Week 3 &amp; 4 (7/6-7/17): Under The Sea</t>
+  </si>
+  <si>
+    <t>Let's go to     Under the Sea</t>
+  </si>
+  <si>
+    <t>*Schedule may change.</t>
+  </si>
+  <si>
+    <t>Week 7 &amp; 8  (8/3-8/14): IAAS Circus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's play          Split the watermellon </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +240,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -254,33 +265,33 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -289,33 +300,33 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -324,21 +335,21 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -346,14 +357,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -440,17 +451,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,7 +540,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="screen">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -835,28 +852,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G6"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="26" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -922,26 +942,26 @@
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A6" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+    <row r="6" spans="1:17" ht="15" thickBot="1">
+      <c r="A6" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
+      <c r="I6" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
@@ -1056,13 +1076,13 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
       <c r="J9" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="M9" s="12" t="s">
         <v>7</v>
@@ -1122,13 +1142,13 @@
         <v>28</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="17">
         <v>30</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" s="7">
         <v>2</v>
@@ -1159,7 +1179,7 @@
         <v>31</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="67.5" customHeight="1" thickBot="1">
@@ -1171,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>7</v>
@@ -1189,36 +1209,36 @@
         <v>7</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>7</v>
       </c>
       <c r="N12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1">
+      <c r="A13" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
+      <c r="I13" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2" t="s">
@@ -1289,7 +1309,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="7">
         <v>3</v>
@@ -1331,7 +1351,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
       <c r="J16" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>7</v>
@@ -1343,7 +1363,7 @@
         <v>7</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="O16" s="10"/>
     </row>
@@ -1446,7 +1466,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>7</v>
@@ -1458,19 +1478,19 @@
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
       <c r="J19" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>7</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O19" s="10"/>
     </row>
@@ -1490,22 +1510,22 @@
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
     </row>
-    <row r="22" spans="1:15" ht="15.75">
-      <c r="B22" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
+    <row r="22" spans="1:15" ht="15">
+      <c r="B22" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1517,32 +1537,48 @@
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="I13:O13"/>
   </mergeCells>
-  <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.2" right="0.19" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup scale="87" orientation="landscape" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>